<commit_message>
Update: Phe duyet bai viet thanh 3 buoc.
</commit_message>
<xml_diff>
--- a/01.CongTTDT/02.Source/HL.Website/Data/upload/files/Incident/Deface/Deface.xlsx
+++ b/01.CongTTDT/02.Source/HL.Website/Data/upload/files/Incident/Deface/Deface.xlsx
@@ -14,12 +14,12 @@
     <sheet name="Attack" sheetId="4" r:id="rId5"/>
     <sheet name="CVE" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Người tấn công</t>
   </si>
@@ -135,91 +135,94 @@
     <t>FPT-VN</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>asn</t>
-  </si>
-  <si>
-    <t>geo</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>type (downadup)</t>
-  </si>
-  <si>
-    <t>http_agent(Mozilla/4.0 (compatible; MSIE 6.0; Windows NT 5.1; SV1))</t>
-  </si>
-  <si>
-    <t>src_port(1938,1499 ...)</t>
-  </si>
-  <si>
-    <t>hostname (static.vnpt.vn, localhost )</t>
-  </si>
-  <si>
-    <t>dst_port (Địa chỉ cổng đích)</t>
-  </si>
-  <si>
-    <t>protocol (udp or tcp)</t>
-  </si>
-  <si>
-    <t>servername</t>
-  </si>
-  <si>
-    <t>server</t>
-  </si>
-  <si>
-    <t>header (HTTP/1.1 200 OK)</t>
-  </si>
-  <si>
-    <t>tag (netis_vulnerability,cwmp,memcached,rdp ...)</t>
-  </si>
-  <si>
-    <t>handshake</t>
-  </si>
-  <si>
-    <t>times</t>
-  </si>
-  <si>
-    <t>attacker IP (tại VN bị nhiễm)</t>
-  </si>
-  <si>
-    <t>network name</t>
-  </si>
-  <si>
-    <t>local IP</t>
-  </si>
-  <si>
-    <t>local TCP port</t>
-  </si>
-  <si>
-    <t>CVE ID</t>
-  </si>
-  <si>
-    <t>Vulnerability Type(s) (Exec Code,DoS CSRF,+Info, XSS ...)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Product </t>
   </si>
   <si>
-    <t>Publish Date</t>
-  </si>
-  <si>
-    <t>Update Date</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
-    <t>Gained Access Level (None)</t>
-  </si>
-  <si>
     <t>http://htec.edu.vn/a.html</t>
   </si>
   <si>
     <t>http://congtynamlimxanh.vn/aaaa/index.html</t>
+  </si>
+  <si>
+    <t>AttackerIP</t>
+  </si>
+  <si>
+    <t>NetwordName</t>
+  </si>
+  <si>
+    <t>LocalIP</t>
+  </si>
+  <si>
+    <t>LocalTCPPort</t>
+  </si>
+  <si>
+    <t>AttankOn</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>ASN</t>
+  </si>
+  <si>
+    <t>Geo</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type </t>
+  </si>
+  <si>
+    <t>HttpAgent</t>
+  </si>
+  <si>
+    <t>SrcPort</t>
+  </si>
+  <si>
+    <t>HostName</t>
+  </si>
+  <si>
+    <t>Destinationport</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>ServerName</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>VulnerabilityType</t>
+  </si>
+  <si>
+    <t>GainedAccessLevel</t>
+  </si>
+  <si>
+    <t>http://congtynamlimxanh.vn/index33.html</t>
+  </si>
+  <si>
+    <t>http://somaco.vn/abc.html</t>
   </si>
 </sst>
 </file>
@@ -250,15 +253,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -266,27 +275,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -294,13 +288,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,16 +621,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -680,7 +678,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -694,7 +692,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -708,7 +706,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -717,6 +715,20 @@
         <v>43131.88958333333</v>
       </c>
       <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43131.303472222222</v>
+      </c>
+      <c r="D8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -728,9 +740,10 @@
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -739,7 +752,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,16 +764,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -822,7 +835,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,22 +849,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -928,128 +941,145 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>57</v>
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="H1" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="C4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1061,41 +1091,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="7" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>64</v>
       </c>
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>